<commit_message>
Update error messages for failed lookups in row data
</commit_message>
<xml_diff>
--- a/tool/test_pack.xlsx
+++ b/tool/test_pack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e\tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{306949C9-326F-40FC-BAA4-AE9525AE9A8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AE7AEC-1B61-48BB-B694-C4C1756BBA49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{7C3F71BD-1F0F-4548-8705-713F65ABAC71}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>Cayston 75mg powder and solvent for nebuliser solution vials with Altera Nebuliser Handset</t>
   </si>
   <si>
-    <t>vials</t>
-  </si>
-  <si>
     <t>nebulise one vial Three times a day for 28 days then alternate with colomycin</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>Sodium chloride 0.9% solution for injection 5ml ampoules</t>
   </si>
   <si>
-    <t>ampoules</t>
-  </si>
-  <si>
     <t>for reconstitution for nebulisation products</t>
   </si>
   <si>
@@ -1004,6 +998,12 @@
   </si>
   <si>
     <t>Prescriber Code</t>
+  </si>
+  <si>
+    <t>vial</t>
+  </si>
+  <si>
+    <t>ampoule</t>
   </si>
 </sst>
 </file>
@@ -1507,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC3E160-3EEC-485C-93B7-9C0F993DBE29}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1533,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1542,13 +1542,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -1574,7 +1574,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C2" s="5">
         <v>1201</v>
@@ -1586,7 +1586,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="5">
         <v>9854001</v>
@@ -1595,7 +1595,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J2" s="5">
         <v>6</v>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C3" s="5">
         <v>1201</v>
@@ -1624,7 +1624,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" s="5">
         <v>9854001</v>
@@ -1633,7 +1633,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J3" s="5">
         <v>24</v>
@@ -1650,7 +1650,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C4" s="5">
         <v>1204</v>
@@ -1662,7 +1662,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5">
         <v>9854001</v>
@@ -1671,16 +1671,16 @@
         <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J4" s="5">
         <v>84</v>
       </c>
       <c r="K4" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1688,7 +1688,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C5" s="5">
         <v>1204</v>
@@ -1700,25 +1700,25 @@
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" s="5">
         <v>9854001</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J5" s="5">
         <v>28</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>16</v>
+        <v>321</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1726,7 +1726,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C6" s="5">
         <v>1204</v>
@@ -1738,25 +1738,25 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G6" s="5">
         <v>9854001</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J6" s="5">
         <v>14</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>21</v>
+        <v>322</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1764,7 +1764,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C7" s="5">
         <v>1208</v>
@@ -1776,25 +1776,25 @@
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="5">
         <v>2080975</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J7" s="5">
         <v>7</v>
       </c>
       <c r="K7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1802,7 +1802,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C8" s="5">
         <v>1208</v>
@@ -1814,25 +1814,25 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G8" s="5">
         <v>2080975</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J8" s="5">
         <v>28</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1934,64 +1934,64 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2005,37 +2005,37 @@
         <v>19480430</v>
       </c>
       <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>56</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>57</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>58</v>
-      </c>
-      <c r="M2" t="s">
-        <v>59</v>
-      </c>
-      <c r="N2" t="s">
-        <v>60</v>
       </c>
       <c r="O2">
         <v>17338054</v>
       </c>
       <c r="Q2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2049,37 +2049,37 @@
         <v>20110330</v>
       </c>
       <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
         <v>63</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" t="s">
         <v>64</v>
       </c>
-      <c r="G3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>57</v>
       </c>
-      <c r="K3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" t="s">
-        <v>59</v>
-      </c>
       <c r="N3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O3">
         <v>17338044</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2093,34 +2093,34 @@
         <v>19850911</v>
       </c>
       <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
         <v>68</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>69</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>70</v>
       </c>
-      <c r="I4" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" t="s">
-        <v>72</v>
-      </c>
       <c r="M4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O4">
         <v>7297494</v>
       </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2134,37 +2134,37 @@
         <v>19940319</v>
       </c>
       <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
         <v>74</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
         <v>75</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>76</v>
       </c>
-      <c r="H5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" t="s">
-        <v>77</v>
-      </c>
-      <c r="K5" t="s">
-        <v>78</v>
-      </c>
       <c r="M5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O5">
         <v>25531063</v>
       </c>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2178,37 +2178,37 @@
         <v>20061217</v>
       </c>
       <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
         <v>80</v>
       </c>
-      <c r="F6" t="s">
+      <c r="K6" t="s">
         <v>81</v>
       </c>
-      <c r="H6" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" t="s">
-        <v>77</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="M6" t="s">
         <v>82</v>
       </c>
-      <c r="K6" t="s">
-        <v>83</v>
-      </c>
-      <c r="M6" t="s">
-        <v>84</v>
-      </c>
       <c r="N6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O6">
         <v>20169633</v>
       </c>
       <c r="Q6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2222,37 +2222,37 @@
         <v>20110113</v>
       </c>
       <c r="E7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" t="s">
         <v>86</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" t="s">
         <v>87</v>
       </c>
-      <c r="G7" t="s">
+      <c r="K7" t="s">
         <v>88</v>
       </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="M7" t="s">
         <v>57</v>
-      </c>
-      <c r="J7" t="s">
-        <v>89</v>
-      </c>
-      <c r="K7" t="s">
-        <v>90</v>
-      </c>
-      <c r="M7" t="s">
-        <v>59</v>
       </c>
       <c r="O7">
         <v>21395494</v>
       </c>
       <c r="Q7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2266,34 +2266,34 @@
         <v>20110614</v>
       </c>
       <c r="E8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
         <v>92</v>
       </c>
-      <c r="F8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>57</v>
       </c>
-      <c r="K8" t="s">
-        <v>94</v>
-      </c>
-      <c r="M8" t="s">
-        <v>59</v>
-      </c>
       <c r="N8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O8">
         <v>7298547</v>
       </c>
       <c r="Q8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2307,37 +2307,37 @@
         <v>19950505</v>
       </c>
       <c r="E9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" t="s">
         <v>96</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" t="s">
         <v>97</v>
       </c>
-      <c r="G9" t="s">
-        <v>98</v>
-      </c>
-      <c r="H9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" t="s">
-        <v>99</v>
-      </c>
       <c r="M9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O9">
         <v>7298187</v>
       </c>
       <c r="Q9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2351,37 +2351,37 @@
         <v>20061108</v>
       </c>
       <c r="E10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" t="s">
         <v>101</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" t="s">
         <v>102</v>
       </c>
-      <c r="G10" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="M10" t="s">
         <v>57</v>
       </c>
-      <c r="K10" t="s">
-        <v>104</v>
-      </c>
-      <c r="M10" t="s">
-        <v>59</v>
-      </c>
       <c r="N10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O10">
         <v>7298003</v>
       </c>
       <c r="Q10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2395,34 +2395,34 @@
         <v>20021025</v>
       </c>
       <c r="E11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" t="s">
         <v>106</v>
       </c>
-      <c r="F11" t="s">
-        <v>107</v>
-      </c>
-      <c r="H11" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" t="s">
-        <v>77</v>
-      </c>
-      <c r="K11" t="s">
-        <v>108</v>
-      </c>
       <c r="M11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O11">
         <v>7297926</v>
       </c>
       <c r="Q11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2436,34 +2436,34 @@
         <v>19941108</v>
       </c>
       <c r="E12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" t="s">
         <v>110</v>
       </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" t="s">
         <v>111</v>
       </c>
-      <c r="H12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="M12" t="s">
         <v>57</v>
       </c>
-      <c r="K12" t="s">
-        <v>113</v>
-      </c>
-      <c r="M12" t="s">
-        <v>59</v>
-      </c>
       <c r="N12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O12">
         <v>7297866</v>
       </c>
       <c r="Q12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2477,37 +2477,37 @@
         <v>20071217</v>
       </c>
       <c r="E13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" t="s">
         <v>115</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>116</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" t="s">
         <v>117</v>
       </c>
-      <c r="H13" t="s">
-        <v>118</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="M13" t="s">
         <v>57</v>
       </c>
-      <c r="K13" t="s">
-        <v>119</v>
-      </c>
-      <c r="M13" t="s">
-        <v>59</v>
-      </c>
       <c r="N13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O13">
         <v>28110363</v>
       </c>
       <c r="Q13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2521,34 +2521,34 @@
         <v>19361013</v>
       </c>
       <c r="E14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" t="s">
         <v>121</v>
       </c>
-      <c r="F14" t="s">
+      <c r="M14" t="s">
         <v>122</v>
       </c>
-      <c r="H14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" t="s">
-        <v>123</v>
-      </c>
-      <c r="M14" t="s">
-        <v>124</v>
-      </c>
       <c r="N14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O14">
         <v>7294854</v>
       </c>
       <c r="Q14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2562,34 +2562,34 @@
         <v>20050104</v>
       </c>
       <c r="E15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" t="s">
         <v>126</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" t="s">
         <v>127</v>
       </c>
-      <c r="G15" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="M15" t="s">
         <v>57</v>
-      </c>
-      <c r="K15" t="s">
-        <v>129</v>
-      </c>
-      <c r="M15" t="s">
-        <v>59</v>
       </c>
       <c r="O15">
         <v>27655636</v>
       </c>
       <c r="Q15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
@@ -2603,34 +2603,34 @@
         <v>20020719</v>
       </c>
       <c r="E16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" t="s">
         <v>131</v>
       </c>
-      <c r="F16" t="s">
-        <v>132</v>
-      </c>
-      <c r="H16" t="s">
-        <v>70</v>
-      </c>
-      <c r="I16" t="s">
-        <v>77</v>
-      </c>
-      <c r="K16" t="s">
-        <v>133</v>
-      </c>
       <c r="M16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O16">
         <v>21971196</v>
       </c>
       <c r="Q16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2644,34 +2644,34 @@
         <v>19920818</v>
       </c>
       <c r="E17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" t="s">
         <v>135</v>
       </c>
-      <c r="F17" t="s">
-        <v>136</v>
-      </c>
-      <c r="H17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K17" t="s">
-        <v>137</v>
-      </c>
       <c r="M17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O17">
         <v>7339558</v>
       </c>
       <c r="Q17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2685,37 +2685,37 @@
         <v>20110601</v>
       </c>
       <c r="E18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" t="s">
         <v>139</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18" t="s">
         <v>140</v>
       </c>
-      <c r="G18" t="s">
+      <c r="L18" t="s">
         <v>141</v>
       </c>
-      <c r="H18" t="s">
-        <v>118</v>
-      </c>
-      <c r="I18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" t="s">
-        <v>142</v>
-      </c>
-      <c r="L18" t="s">
-        <v>143</v>
-      </c>
       <c r="M18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O18">
         <v>7292938</v>
       </c>
       <c r="Q18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2729,40 +2729,40 @@
         <v>19031104</v>
       </c>
       <c r="E19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" t="s">
+        <v>144</v>
+      </c>
+      <c r="G19" t="s">
         <v>145</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" t="s">
         <v>146</v>
       </c>
-      <c r="G19" t="s">
-        <v>147</v>
-      </c>
-      <c r="H19" t="s">
-        <v>70</v>
-      </c>
-      <c r="I19" t="s">
-        <v>77</v>
-      </c>
-      <c r="K19" t="s">
-        <v>148</v>
-      </c>
       <c r="L19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O19">
         <v>7292919</v>
       </c>
       <c r="Q19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2776,40 +2776,40 @@
         <v>20110628</v>
       </c>
       <c r="E20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F20" t="s">
+        <v>149</v>
+      </c>
+      <c r="G20" t="s">
         <v>150</v>
       </c>
-      <c r="F20" t="s">
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" t="s">
         <v>151</v>
       </c>
-      <c r="G20" t="s">
-        <v>152</v>
-      </c>
-      <c r="H20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" t="s">
-        <v>57</v>
-      </c>
-      <c r="K20" t="s">
-        <v>153</v>
-      </c>
       <c r="L20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O20">
         <v>7292789</v>
       </c>
       <c r="Q20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2823,37 +2823,37 @@
         <v>20060928</v>
       </c>
       <c r="E21" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" t="s">
+        <v>154</v>
+      </c>
+      <c r="H21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" t="s">
         <v>155</v>
       </c>
-      <c r="F21" t="s">
+      <c r="K21" t="s">
         <v>156</v>
       </c>
-      <c r="H21" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" t="s">
-        <v>77</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="L21" t="s">
         <v>157</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>158</v>
-      </c>
-      <c r="L21" t="s">
-        <v>159</v>
-      </c>
-      <c r="M21" t="s">
-        <v>160</v>
       </c>
       <c r="O21">
         <v>21852494</v>
       </c>
       <c r="Q21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2867,34 +2867,34 @@
         <v>20040426</v>
       </c>
       <c r="E22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F22" t="s">
+        <v>161</v>
+      </c>
+      <c r="H22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I22" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" t="s">
         <v>162</v>
       </c>
-      <c r="F22" t="s">
+      <c r="K22" t="s">
         <v>163</v>
       </c>
-      <c r="H22" t="s">
-        <v>118</v>
-      </c>
-      <c r="I22" t="s">
-        <v>57</v>
-      </c>
-      <c r="J22" t="s">
-        <v>164</v>
-      </c>
-      <c r="K22" t="s">
-        <v>165</v>
-      </c>
       <c r="M22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O22">
         <v>19911060</v>
       </c>
       <c r="Q22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2908,37 +2908,37 @@
         <v>20030901</v>
       </c>
       <c r="E23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" t="s">
+        <v>166</v>
+      </c>
+      <c r="H23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" t="s">
         <v>167</v>
       </c>
-      <c r="F23" t="s">
+      <c r="K23" t="s">
         <v>168</v>
       </c>
-      <c r="H23" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" t="s">
-        <v>71</v>
-      </c>
-      <c r="J23" t="s">
-        <v>169</v>
-      </c>
-      <c r="K23" t="s">
-        <v>170</v>
-      </c>
       <c r="L23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O23">
         <v>21852491</v>
       </c>
       <c r="Q23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2952,31 +2952,31 @@
         <v>19490108</v>
       </c>
       <c r="E24" t="s">
+        <v>170</v>
+      </c>
+      <c r="F24" t="s">
+        <v>171</v>
+      </c>
+      <c r="H24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K24" t="s">
         <v>172</v>
       </c>
-      <c r="F24" t="s">
-        <v>173</v>
-      </c>
-      <c r="H24" t="s">
-        <v>70</v>
-      </c>
-      <c r="I24" t="s">
-        <v>77</v>
-      </c>
-      <c r="K24" t="s">
-        <v>174</v>
-      </c>
       <c r="M24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O24">
         <v>16406373</v>
       </c>
       <c r="Q24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2990,34 +2990,34 @@
         <v>20110429</v>
       </c>
       <c r="E25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" t="s">
         <v>176</v>
       </c>
-      <c r="F25" t="s">
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K25" t="s">
         <v>177</v>
       </c>
-      <c r="G25" t="s">
-        <v>178</v>
-      </c>
-      <c r="H25" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" t="s">
-        <v>57</v>
-      </c>
-      <c r="K25" t="s">
-        <v>179</v>
-      </c>
       <c r="M25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O25">
         <v>32115549</v>
       </c>
       <c r="Q25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3031,40 +3031,40 @@
         <v>20110131</v>
       </c>
       <c r="E26" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" t="s">
+        <v>180</v>
+      </c>
+      <c r="G26" t="s">
         <v>181</v>
       </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" t="s">
         <v>182</v>
       </c>
-      <c r="G26" t="s">
+      <c r="K26" t="s">
         <v>183</v>
       </c>
-      <c r="H26" t="s">
-        <v>56</v>
-      </c>
-      <c r="I26" t="s">
-        <v>71</v>
-      </c>
-      <c r="J26" t="s">
-        <v>184</v>
-      </c>
-      <c r="K26" t="s">
-        <v>185</v>
-      </c>
       <c r="L26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O26">
         <v>16406248</v>
       </c>
       <c r="Q26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3078,37 +3078,37 @@
         <v>19490907</v>
       </c>
       <c r="E27" t="s">
+        <v>185</v>
+      </c>
+      <c r="F27" t="s">
+        <v>186</v>
+      </c>
+      <c r="H27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27" t="s">
         <v>187</v>
       </c>
-      <c r="F27" t="s">
-        <v>188</v>
-      </c>
-      <c r="H27" t="s">
-        <v>70</v>
-      </c>
-      <c r="I27" t="s">
-        <v>71</v>
-      </c>
-      <c r="K27" t="s">
-        <v>189</v>
-      </c>
       <c r="L27" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O27">
         <v>7293033</v>
       </c>
       <c r="Q27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3122,37 +3122,37 @@
         <v>20090325</v>
       </c>
       <c r="E28" t="s">
+        <v>189</v>
+      </c>
+      <c r="F28" t="s">
+        <v>190</v>
+      </c>
+      <c r="G28" t="s">
         <v>191</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" t="s">
         <v>192</v>
       </c>
-      <c r="G28" t="s">
-        <v>193</v>
-      </c>
-      <c r="H28" t="s">
-        <v>56</v>
-      </c>
-      <c r="I28" t="s">
-        <v>57</v>
-      </c>
-      <c r="K28" t="s">
-        <v>194</v>
-      </c>
       <c r="M28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O28">
         <v>7339972</v>
       </c>
       <c r="Q28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3166,37 +3166,37 @@
         <v>19260501</v>
       </c>
       <c r="E29" t="s">
+        <v>194</v>
+      </c>
+      <c r="F29" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" t="s">
         <v>196</v>
       </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
+        <v>110</v>
+      </c>
+      <c r="I29" t="s">
+        <v>55</v>
+      </c>
+      <c r="K29" t="s">
         <v>197</v>
       </c>
-      <c r="G29" t="s">
-        <v>198</v>
-      </c>
-      <c r="H29" t="s">
-        <v>112</v>
-      </c>
-      <c r="I29" t="s">
-        <v>57</v>
-      </c>
-      <c r="K29" t="s">
-        <v>199</v>
-      </c>
       <c r="M29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O29">
         <v>7339913</v>
       </c>
       <c r="Q29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3210,40 +3210,40 @@
         <v>20110314</v>
       </c>
       <c r="E30" t="s">
+        <v>199</v>
+      </c>
+      <c r="F30" t="s">
+        <v>200</v>
+      </c>
+      <c r="G30" t="s">
         <v>201</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" t="s">
         <v>202</v>
       </c>
-      <c r="G30" t="s">
+      <c r="J30" t="s">
         <v>203</v>
       </c>
-      <c r="H30" t="s">
-        <v>70</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="K30" t="s">
         <v>204</v>
       </c>
-      <c r="J30" t="s">
-        <v>205</v>
-      </c>
-      <c r="K30" t="s">
-        <v>206</v>
-      </c>
       <c r="L30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O30">
         <v>16406199</v>
       </c>
       <c r="Q30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3257,40 +3257,40 @@
         <v>20110221</v>
       </c>
       <c r="E31" t="s">
+        <v>206</v>
+      </c>
+      <c r="F31" t="s">
+        <v>207</v>
+      </c>
+      <c r="G31" t="s">
         <v>208</v>
       </c>
-      <c r="F31" t="s">
+      <c r="H31" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" t="s">
         <v>209</v>
       </c>
-      <c r="G31" t="s">
-        <v>210</v>
-      </c>
-      <c r="H31" t="s">
-        <v>70</v>
-      </c>
-      <c r="I31" t="s">
-        <v>77</v>
-      </c>
-      <c r="J31" t="s">
-        <v>211</v>
-      </c>
       <c r="K31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O31">
         <v>16406190</v>
       </c>
       <c r="Q31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3304,37 +3304,37 @@
         <v>20110304</v>
       </c>
       <c r="E32" t="s">
+        <v>211</v>
+      </c>
+      <c r="F32" t="s">
+        <v>212</v>
+      </c>
+      <c r="H32" t="s">
+        <v>68</v>
+      </c>
+      <c r="I32" t="s">
+        <v>75</v>
+      </c>
+      <c r="J32" t="s">
         <v>213</v>
       </c>
-      <c r="F32" t="s">
+      <c r="K32" t="s">
         <v>214</v>
       </c>
-      <c r="H32" t="s">
-        <v>70</v>
-      </c>
-      <c r="I32" t="s">
-        <v>77</v>
-      </c>
-      <c r="J32" t="s">
-        <v>215</v>
-      </c>
-      <c r="K32" t="s">
-        <v>216</v>
-      </c>
       <c r="L32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O32">
         <v>16406143</v>
       </c>
       <c r="Q32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3348,37 +3348,37 @@
         <v>20071004</v>
       </c>
       <c r="E33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F33" t="s">
+        <v>217</v>
+      </c>
+      <c r="H33" t="s">
+        <v>68</v>
+      </c>
+      <c r="I33" t="s">
+        <v>75</v>
+      </c>
+      <c r="J33" t="s">
         <v>218</v>
       </c>
-      <c r="F33" t="s">
-        <v>219</v>
-      </c>
-      <c r="H33" t="s">
-        <v>70</v>
-      </c>
-      <c r="I33" t="s">
-        <v>77</v>
-      </c>
-      <c r="J33" t="s">
-        <v>220</v>
-      </c>
       <c r="K33" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="L33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M33" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O33">
         <v>16406137</v>
       </c>
       <c r="Q33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S33" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3392,37 +3392,37 @@
         <v>19391003</v>
       </c>
       <c r="E34" t="s">
+        <v>220</v>
+      </c>
+      <c r="F34" t="s">
+        <v>221</v>
+      </c>
+      <c r="G34" t="s">
         <v>222</v>
       </c>
-      <c r="F34" t="s">
+      <c r="H34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I34" t="s">
+        <v>55</v>
+      </c>
+      <c r="K34" t="s">
         <v>223</v>
       </c>
-      <c r="G34" t="s">
-        <v>224</v>
-      </c>
-      <c r="H34" t="s">
-        <v>118</v>
-      </c>
-      <c r="I34" t="s">
-        <v>57</v>
-      </c>
-      <c r="K34" t="s">
-        <v>225</v>
-      </c>
       <c r="L34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O34">
         <v>3039778</v>
       </c>
       <c r="Q34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S34" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3436,37 +3436,37 @@
         <v>19650906</v>
       </c>
       <c r="E35" t="s">
+        <v>225</v>
+      </c>
+      <c r="F35" t="s">
+        <v>226</v>
+      </c>
+      <c r="G35" t="s">
         <v>227</v>
       </c>
-      <c r="F35" t="s">
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" t="s">
+        <v>75</v>
+      </c>
+      <c r="K35" t="s">
         <v>228</v>
       </c>
-      <c r="G35" t="s">
-        <v>229</v>
-      </c>
-      <c r="H35" t="s">
-        <v>70</v>
-      </c>
-      <c r="I35" t="s">
-        <v>77</v>
-      </c>
-      <c r="K35" t="s">
-        <v>230</v>
-      </c>
       <c r="L35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O35">
         <v>23874432</v>
       </c>
       <c r="Q35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S35" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3480,43 +3480,43 @@
         <v>20100716</v>
       </c>
       <c r="E36" t="s">
+        <v>230</v>
+      </c>
+      <c r="F36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G36" t="s">
         <v>232</v>
       </c>
-      <c r="F36" t="s">
+      <c r="H36" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" t="s">
         <v>233</v>
       </c>
-      <c r="G36" t="s">
+      <c r="K36" t="s">
         <v>234</v>
       </c>
-      <c r="H36" t="s">
-        <v>56</v>
-      </c>
-      <c r="I36" t="s">
-        <v>57</v>
-      </c>
-      <c r="J36" t="s">
-        <v>235</v>
-      </c>
-      <c r="K36" t="s">
-        <v>236</v>
-      </c>
       <c r="L36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O36">
         <v>21261329</v>
       </c>
       <c r="Q36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S36" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3530,40 +3530,40 @@
         <v>19590820</v>
       </c>
       <c r="E37" t="s">
+        <v>236</v>
+      </c>
+      <c r="F37" t="s">
+        <v>237</v>
+      </c>
+      <c r="G37" t="s">
         <v>238</v>
       </c>
-      <c r="F37" t="s">
+      <c r="H37" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" t="s">
+        <v>75</v>
+      </c>
+      <c r="K37" t="s">
         <v>239</v>
       </c>
-      <c r="G37" t="s">
-        <v>240</v>
-      </c>
-      <c r="H37" t="s">
-        <v>70</v>
-      </c>
-      <c r="I37" t="s">
-        <v>77</v>
-      </c>
-      <c r="K37" t="s">
-        <v>241</v>
-      </c>
       <c r="L37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M37" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O37">
         <v>7294294</v>
       </c>
       <c r="Q37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S37" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3577,37 +3577,37 @@
         <v>20110614</v>
       </c>
       <c r="E38" t="s">
+        <v>241</v>
+      </c>
+      <c r="F38" t="s">
+        <v>242</v>
+      </c>
+      <c r="H38" t="s">
+        <v>68</v>
+      </c>
+      <c r="I38" t="s">
+        <v>75</v>
+      </c>
+      <c r="J38" t="s">
         <v>243</v>
       </c>
-      <c r="F38" t="s">
+      <c r="K38" t="s">
         <v>244</v>
       </c>
-      <c r="H38" t="s">
-        <v>70</v>
-      </c>
-      <c r="I38" t="s">
-        <v>77</v>
-      </c>
-      <c r="J38" t="s">
-        <v>245</v>
-      </c>
-      <c r="K38" t="s">
-        <v>246</v>
-      </c>
       <c r="L38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O38">
         <v>16406287</v>
       </c>
       <c r="Q38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S38" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3621,37 +3621,37 @@
         <v>19970706</v>
       </c>
       <c r="E39" t="s">
+        <v>246</v>
+      </c>
+      <c r="F39" t="s">
+        <v>247</v>
+      </c>
+      <c r="G39" t="s">
         <v>248</v>
       </c>
-      <c r="F39" t="s">
+      <c r="H39" t="s">
+        <v>54</v>
+      </c>
+      <c r="I39" t="s">
+        <v>55</v>
+      </c>
+      <c r="K39" t="s">
         <v>249</v>
       </c>
-      <c r="G39" t="s">
-        <v>250</v>
-      </c>
-      <c r="H39" t="s">
-        <v>56</v>
-      </c>
-      <c r="I39" t="s">
-        <v>57</v>
-      </c>
-      <c r="K39" t="s">
-        <v>251</v>
-      </c>
       <c r="M39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O39">
         <v>7294713</v>
       </c>
       <c r="Q39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S39" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3665,37 +3665,37 @@
         <v>20100202</v>
       </c>
       <c r="E40" t="s">
+        <v>251</v>
+      </c>
+      <c r="F40" t="s">
+        <v>252</v>
+      </c>
+      <c r="G40" t="s">
         <v>253</v>
       </c>
-      <c r="F40" t="s">
+      <c r="H40" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" t="s">
+        <v>55</v>
+      </c>
+      <c r="K40" t="s">
         <v>254</v>
       </c>
-      <c r="G40" t="s">
-        <v>255</v>
-      </c>
-      <c r="H40" t="s">
-        <v>56</v>
-      </c>
-      <c r="I40" t="s">
-        <v>57</v>
-      </c>
-      <c r="K40" t="s">
-        <v>256</v>
-      </c>
       <c r="M40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O40">
         <v>7342624</v>
       </c>
       <c r="Q40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S40" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3709,37 +3709,37 @@
         <v>20010414</v>
       </c>
       <c r="E41" t="s">
+        <v>256</v>
+      </c>
+      <c r="F41" t="s">
+        <v>257</v>
+      </c>
+      <c r="G41" t="s">
         <v>258</v>
       </c>
-      <c r="F41" t="s">
+      <c r="H41" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" t="s">
+        <v>75</v>
+      </c>
+      <c r="K41" t="s">
         <v>259</v>
       </c>
-      <c r="G41" t="s">
-        <v>260</v>
-      </c>
-      <c r="H41" t="s">
-        <v>70</v>
-      </c>
-      <c r="I41" t="s">
-        <v>77</v>
-      </c>
-      <c r="K41" t="s">
-        <v>261</v>
-      </c>
       <c r="M41" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O41">
         <v>7294680</v>
       </c>
       <c r="Q41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S41" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3753,37 +3753,37 @@
         <v>20101221</v>
       </c>
       <c r="E42" t="s">
+        <v>261</v>
+      </c>
+      <c r="F42" t="s">
+        <v>262</v>
+      </c>
+      <c r="G42" t="s">
         <v>263</v>
       </c>
-      <c r="F42" t="s">
+      <c r="H42" t="s">
+        <v>54</v>
+      </c>
+      <c r="I42" t="s">
+        <v>55</v>
+      </c>
+      <c r="K42" t="s">
         <v>264</v>
       </c>
-      <c r="G42" t="s">
-        <v>265</v>
-      </c>
-      <c r="H42" t="s">
-        <v>56</v>
-      </c>
-      <c r="I42" t="s">
-        <v>57</v>
-      </c>
-      <c r="K42" t="s">
-        <v>266</v>
-      </c>
       <c r="M42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N42" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O42">
         <v>7294344</v>
       </c>
       <c r="Q42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S42" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3797,37 +3797,37 @@
         <v>19670906</v>
       </c>
       <c r="E43" t="s">
+        <v>266</v>
+      </c>
+      <c r="F43" t="s">
+        <v>267</v>
+      </c>
+      <c r="G43" t="s">
         <v>268</v>
       </c>
-      <c r="F43" t="s">
+      <c r="H43" t="s">
+        <v>54</v>
+      </c>
+      <c r="I43" t="s">
+        <v>202</v>
+      </c>
+      <c r="K43" t="s">
         <v>269</v>
       </c>
-      <c r="G43" t="s">
-        <v>270</v>
-      </c>
-      <c r="H43" t="s">
-        <v>56</v>
-      </c>
-      <c r="I43" t="s">
-        <v>204</v>
-      </c>
-      <c r="K43" t="s">
-        <v>271</v>
-      </c>
       <c r="M43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O43">
         <v>7294343</v>
       </c>
       <c r="Q43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S43" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3841,37 +3841,37 @@
         <v>20100809</v>
       </c>
       <c r="E44" t="s">
+        <v>270</v>
+      </c>
+      <c r="F44" t="s">
+        <v>271</v>
+      </c>
+      <c r="G44" t="s">
         <v>272</v>
       </c>
-      <c r="F44" t="s">
+      <c r="H44" t="s">
+        <v>68</v>
+      </c>
+      <c r="I44" t="s">
+        <v>75</v>
+      </c>
+      <c r="K44" t="s">
         <v>273</v>
       </c>
-      <c r="G44" t="s">
-        <v>274</v>
-      </c>
-      <c r="H44" t="s">
-        <v>70</v>
-      </c>
-      <c r="I44" t="s">
-        <v>77</v>
-      </c>
-      <c r="K44" t="s">
-        <v>275</v>
-      </c>
       <c r="M44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O44">
         <v>7294331</v>
       </c>
       <c r="Q44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S44" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3885,40 +3885,40 @@
         <v>20070720</v>
       </c>
       <c r="E45" t="s">
+        <v>275</v>
+      </c>
+      <c r="F45" t="s">
+        <v>276</v>
+      </c>
+      <c r="G45" t="s">
         <v>277</v>
       </c>
-      <c r="F45" t="s">
+      <c r="H45" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" t="s">
+        <v>75</v>
+      </c>
+      <c r="K45" t="s">
         <v>278</v>
       </c>
-      <c r="G45" t="s">
-        <v>279</v>
-      </c>
-      <c r="H45" t="s">
-        <v>70</v>
-      </c>
-      <c r="I45" t="s">
-        <v>77</v>
-      </c>
-      <c r="K45" t="s">
-        <v>280</v>
-      </c>
       <c r="L45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M45" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O45">
         <v>7294300</v>
       </c>
       <c r="Q45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S45" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3932,40 +3932,40 @@
         <v>19970307</v>
       </c>
       <c r="E46" t="s">
+        <v>280</v>
+      </c>
+      <c r="F46" t="s">
+        <v>281</v>
+      </c>
+      <c r="G46" t="s">
         <v>282</v>
       </c>
-      <c r="F46" t="s">
+      <c r="H46" t="s">
+        <v>54</v>
+      </c>
+      <c r="I46" t="s">
+        <v>55</v>
+      </c>
+      <c r="K46" t="s">
         <v>283</v>
       </c>
-      <c r="G46" t="s">
-        <v>284</v>
-      </c>
-      <c r="H46" t="s">
-        <v>56</v>
-      </c>
-      <c r="I46" t="s">
-        <v>57</v>
-      </c>
-      <c r="K46" t="s">
-        <v>285</v>
-      </c>
       <c r="L46" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M46" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N46" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O46">
         <v>7293237</v>
       </c>
       <c r="Q46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S46" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -3979,37 +3979,37 @@
         <v>20100814</v>
       </c>
       <c r="E47" t="s">
+        <v>285</v>
+      </c>
+      <c r="F47" t="s">
+        <v>286</v>
+      </c>
+      <c r="H47" t="s">
+        <v>54</v>
+      </c>
+      <c r="I47" t="s">
+        <v>55</v>
+      </c>
+      <c r="K47" t="s">
         <v>287</v>
       </c>
-      <c r="F47" t="s">
-        <v>288</v>
-      </c>
-      <c r="H47" t="s">
-        <v>56</v>
-      </c>
-      <c r="I47" t="s">
-        <v>57</v>
-      </c>
-      <c r="K47" t="s">
-        <v>289</v>
-      </c>
       <c r="L47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N47" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O47">
         <v>17335951</v>
       </c>
       <c r="Q47" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S47" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -4023,34 +4023,34 @@
         <v>20090808</v>
       </c>
       <c r="E48" t="s">
+        <v>289</v>
+      </c>
+      <c r="F48" t="s">
+        <v>290</v>
+      </c>
+      <c r="H48" t="s">
+        <v>54</v>
+      </c>
+      <c r="I48" t="s">
+        <v>55</v>
+      </c>
+      <c r="K48" t="s">
         <v>291</v>
       </c>
-      <c r="F48" t="s">
-        <v>292</v>
-      </c>
-      <c r="H48" t="s">
-        <v>56</v>
-      </c>
-      <c r="I48" t="s">
-        <v>57</v>
-      </c>
-      <c r="K48" t="s">
-        <v>293</v>
-      </c>
       <c r="M48" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N48" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O48">
         <v>17336387</v>
       </c>
       <c r="Q48" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S48" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -4064,37 +4064,37 @@
         <v>20000915</v>
       </c>
       <c r="E49" t="s">
+        <v>293</v>
+      </c>
+      <c r="F49" t="s">
+        <v>294</v>
+      </c>
+      <c r="H49" t="s">
+        <v>68</v>
+      </c>
+      <c r="I49" t="s">
+        <v>75</v>
+      </c>
+      <c r="K49" t="s">
         <v>295</v>
       </c>
-      <c r="F49" t="s">
-        <v>296</v>
-      </c>
-      <c r="H49" t="s">
-        <v>70</v>
-      </c>
-      <c r="I49" t="s">
-        <v>77</v>
-      </c>
-      <c r="K49" t="s">
-        <v>297</v>
-      </c>
       <c r="L49" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M49" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N49" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O49">
         <v>23376110</v>
       </c>
       <c r="Q49" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S49" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -4108,37 +4108,37 @@
         <v>20100914</v>
       </c>
       <c r="E50" t="s">
+        <v>297</v>
+      </c>
+      <c r="F50" t="s">
+        <v>298</v>
+      </c>
+      <c r="H50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I50" t="s">
+        <v>75</v>
+      </c>
+      <c r="K50" t="s">
         <v>299</v>
       </c>
-      <c r="F50" t="s">
-        <v>300</v>
-      </c>
-      <c r="H50" t="s">
-        <v>70</v>
-      </c>
-      <c r="I50" t="s">
-        <v>77</v>
-      </c>
-      <c r="K50" t="s">
-        <v>301</v>
-      </c>
       <c r="L50" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M50" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O50">
         <v>30544647</v>
       </c>
       <c r="Q50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S50" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -4152,37 +4152,37 @@
         <v>19330712</v>
       </c>
       <c r="E51" t="s">
+        <v>301</v>
+      </c>
+      <c r="F51" t="s">
+        <v>302</v>
+      </c>
+      <c r="G51" t="s">
         <v>303</v>
       </c>
-      <c r="F51" t="s">
+      <c r="H51" t="s">
+        <v>68</v>
+      </c>
+      <c r="I51" t="s">
+        <v>75</v>
+      </c>
+      <c r="K51" t="s">
         <v>304</v>
       </c>
-      <c r="G51" t="s">
-        <v>305</v>
-      </c>
-      <c r="H51" t="s">
-        <v>70</v>
-      </c>
-      <c r="I51" t="s">
-        <v>77</v>
-      </c>
-      <c r="K51" t="s">
-        <v>306</v>
-      </c>
       <c r="M51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N51" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O51">
         <v>7342295</v>
       </c>
       <c r="Q51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S51" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -4196,37 +4196,37 @@
         <v>20101126</v>
       </c>
       <c r="E52" t="s">
+        <v>306</v>
+      </c>
+      <c r="F52" t="s">
+        <v>307</v>
+      </c>
+      <c r="H52" t="s">
+        <v>54</v>
+      </c>
+      <c r="I52" t="s">
+        <v>55</v>
+      </c>
+      <c r="K52" t="s">
         <v>308</v>
       </c>
-      <c r="F52" t="s">
-        <v>309</v>
-      </c>
-      <c r="H52" t="s">
-        <v>56</v>
-      </c>
-      <c r="I52" t="s">
-        <v>57</v>
-      </c>
-      <c r="K52" t="s">
-        <v>310</v>
-      </c>
       <c r="L52" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M52" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O52">
         <v>7293589</v>
       </c>
       <c r="Q52" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S52" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Null handling for multiline fields, more encapsulation
</commit_message>
<xml_diff>
--- a/tool/test_pack.xlsx
+++ b/tool/test_pack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e\tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AE7AEC-1B61-48BB-B694-C4C1756BBA49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A8C892-E101-4F3C-8340-DEF7DC85FCA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{7C3F71BD-1F0F-4548-8705-713F65ABAC71}"/>
   </bookViews>
@@ -1507,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC3E160-3EEC-485C-93B7-9C0F993DBE29}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>